<commit_message>
Using Custom Date Formating.
</commit_message>
<xml_diff>
--- a/01.Monthly_Budget.xlsx
+++ b/01.Monthly_Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\002HAW744\Desktop\Personal Projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAA9DA3-96CD-4105-BFA5-3A498B7E0EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08830196-19E3-459B-BF9F-5826BD6E1554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7695" yWindow="346" windowWidth="14423" windowHeight="10782" xr2:uid="{AAA0E821-4CEA-4987-BC7A-3FFF59E41F5E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -64,6 +64,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="mmm/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,7 +98,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,18 +413,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724E3CB5-735B-4659-920B-B1B8C6B7B9BC}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -517,7 +520,13 @@
         <v>125</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring 01.Monthly_Budget.xlsx Using SUM Function.
</commit_message>
<xml_diff>
--- a/01.Monthly_Budget.xlsx
+++ b/01.Monthly_Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\002HAW744\Desktop\Personal Projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8C2701-14FB-4953-8B9F-2FC4CAE0C9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DCB129-4351-49FD-9AEB-65BC449E84D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7695" yWindow="346" windowWidth="14423" windowHeight="10782" xr2:uid="{AAA0E821-4CEA-4987-BC7A-3FFF59E41F5E}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +470,7 @@
         <v>1000</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E9" si="0">B4+C4+D4</f>
+        <f>SUM(B4:D4)</f>
         <v>3000</v>
       </c>
       <c r="F4">
@@ -492,11 +492,11 @@
         <v>100</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E5:E8" si="0">SUM(B5:D5)</f>
         <v>350</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F9" si="1">E5/$E$9</f>
+        <f>E5/$E$9</f>
         <v>6.8292682926829273E-2</v>
       </c>
     </row>
@@ -518,7 +518,7 @@
         <v>525</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f>E6/$E$9</f>
         <v>0.1024390243902439</v>
       </c>
     </row>
@@ -540,7 +540,7 @@
         <v>925</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f>E7/$E$9</f>
         <v>0.18048780487804877</v>
       </c>
     </row>
@@ -562,7 +562,7 @@
         <v>325</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f>E8/$E$9</f>
         <v>6.3414634146341464E-2</v>
       </c>
     </row>
@@ -571,23 +571,23 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <f>B4+B5+B6+B7+B8</f>
+        <f>SUM(B4:B8)</f>
         <v>1675</v>
       </c>
       <c r="C9">
-        <f>C4+C5+C6+C7+C8</f>
+        <f t="shared" ref="C9:E9" si="1">SUM(C4:C8)</f>
         <v>1700</v>
       </c>
       <c r="D9">
-        <f>D4+D5+D6+D7+D8</f>
+        <f t="shared" si="1"/>
         <v>1750</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5125</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f>E9/$E$9</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Using Min and Max Function.
</commit_message>
<xml_diff>
--- a/01.Monthly_Budget.xlsx
+++ b/01.Monthly_Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\002HAW744\Desktop\Personal Projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DCB129-4351-49FD-9AEB-65BC449E84D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49964E52-BC02-4CBE-BECA-2D0DDD9A06AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7695" yWindow="346" windowWidth="14423" windowHeight="10782" xr2:uid="{AAA0E821-4CEA-4987-BC7A-3FFF59E41F5E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>Minimum Expense</t>
+  </si>
+  <si>
+    <t>Maximum Expense</t>
   </si>
 </sst>
 </file>
@@ -416,19 +422,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724E3CB5-735B-4659-920B-B1B8C6B7B9BC}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -591,6 +598,56 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <f>MIN(B4:B8)</f>
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:F12" si="2">MIN(C4:C8)</f>
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>325</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>6.3414634146341464E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <f>MAX(B4:B8)</f>
+        <v>1000</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:F13" si="3">MAX(C4:C8)</f>
+        <v>1000</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>3000</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>0.58536585365853655</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Using Count and Average Function.
</commit_message>
<xml_diff>
--- a/01.Monthly_Budget.xlsx
+++ b/01.Monthly_Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\002HAW744\Desktop\Personal Projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49964E52-BC02-4CBE-BECA-2D0DDD9A06AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7853B1C5-B62A-48CD-AC5F-CDA86C73CD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7695" yWindow="346" windowWidth="14423" windowHeight="10782" xr2:uid="{AAA0E821-4CEA-4987-BC7A-3FFF59E41F5E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Monthly Budget</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Maximum Expense</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724E3CB5-735B-4659-920B-B1B8C6B7B9BC}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,6 +654,56 @@
         <v>0.58536585365853655</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <f>AVERAGE(B4:B8)</f>
+        <v>335</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:F14" si="4">AVERAGE(C4:C8)</f>
+        <v>340</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>1025</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <f>COUNT(B4:B8)</f>
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:F15" si="5">COUNT(C4:C8)</f>
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Using Autosum shortcut key.
</commit_message>
<xml_diff>
--- a/01.Monthly_Budget.xlsx
+++ b/01.Monthly_Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\002HAW744\Desktop\Personal Projects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7853B1C5-B62A-48CD-AC5F-CDA86C73CD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9819BD52-5E84-469E-821A-0D60C2C23A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7695" yWindow="346" windowWidth="14423" windowHeight="10782" xr2:uid="{AAA0E821-4CEA-4987-BC7A-3FFF59E41F5E}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,7 +483,7 @@
         <v>1000</v>
       </c>
       <c r="E4">
-        <f>SUM(B4:D4)</f>
+        <f t="shared" ref="E4:E8" si="0">SUM(B4:D4)</f>
         <v>3000</v>
       </c>
       <c r="F4">
@@ -505,7 +505,7 @@
         <v>100</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E8" si="0">SUM(B5:D5)</f>
+        <f t="shared" si="0"/>
         <v>350</v>
       </c>
       <c r="F5">
@@ -592,7 +592,7 @@
         <v>1700</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f>SUM(D4:D8)</f>
         <v>1750</v>
       </c>
       <c r="E9">
@@ -613,7 +613,7 @@
         <v>100</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:F12" si="2">MIN(C4:C8)</f>
+        <f t="shared" ref="C12:D12" si="2">MIN(C4:C8)</f>
         <v>100</v>
       </c>
       <c r="D12">
@@ -621,11 +621,11 @@
         <v>100</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C12:F12" si="3">MIN(E4:E8)</f>
         <v>325</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3414634146341464E-2</v>
       </c>
     </row>
@@ -638,19 +638,19 @@
         <v>1000</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:F13" si="3">MAX(C4:C8)</f>
+        <f t="shared" ref="C13:F13" si="4">MAX(C4:C8)</f>
         <v>1000</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000</v>
       </c>
       <c r="E13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3000</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.58536585365853655</v>
       </c>
     </row>
@@ -663,19 +663,19 @@
         <v>335</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:F14" si="4">AVERAGE(C4:C8)</f>
+        <f t="shared" ref="C14:F14" si="5">AVERAGE(C4:C8)</f>
         <v>340</v>
       </c>
       <c r="D14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>350</v>
       </c>
       <c r="E14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1025</v>
       </c>
       <c r="F14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
     </row>
@@ -688,24 +688,27 @@
         <v>5</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:F15" si="5">COUNT(C4:C8)</f>
+        <f t="shared" ref="C15:F15" si="6">COUNT(C4:C8)</f>
         <v>5</v>
       </c>
       <c r="D15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="E15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="F15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B12:D15 B9:D9" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>